<commit_message>
Updated experiment lx iteration
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Lx_Parameters_Estimation/1-Trained-Models/Iteration-Results/test_lsb.xlsx
+++ b/Parameters-Estimation/Lx_Parameters_Estimation/1-Trained-Models/Iteration-Results/test_lsb.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>RMSE</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Corr Coeff</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="true"/>
@@ -87,8 +90,9 @@
     <col min="3" max="3" width="12.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
-    <col min="6" max="6" width="12.7109375" customWidth="true"/>
-    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="6" max="6" width="13.42578125" customWidth="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -113,120 +117,138 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>3.1048054984892164</v>
+        <v>4.4210263244707022</v>
       </c>
       <c r="B2" s="0">
-        <v>2.9817801550455902</v>
+        <v>3.1546950902821074</v>
       </c>
       <c r="C2" s="0">
-        <v>0.4719293259433317</v>
+        <v>0.41146286843744595</v>
       </c>
       <c r="D2" s="0">
-        <v>0.68697112453387132</v>
+        <v>0.64145371496113879</v>
       </c>
       <c r="E2" s="0">
-        <v>0.81737394601030422</v>
+        <v>0.54316375521386151</v>
       </c>
       <c r="F2" s="0">
-        <v>0.5280706740566683</v>
+        <v>0.58853713156255405</v>
       </c>
       <c r="G2" s="0">
-        <v>0.9735924240448719</v>
+        <v>0.77377551794237132</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0.28087841959788457</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2.3373067225280644</v>
+        <v>4.9643016717198858</v>
       </c>
       <c r="B3" s="0">
-        <v>2.1353146514981916</v>
+        <v>4.1375026227856795</v>
       </c>
       <c r="C3" s="0">
-        <v>0.42693050290519552</v>
+        <v>1.1106234942423863</v>
       </c>
       <c r="D3" s="0">
-        <v>0.65339919108091615</v>
+        <v>1.0538612310178159</v>
       </c>
       <c r="E3" s="0">
-        <v>0.62073100334249753</v>
+        <v>1.107468582116081</v>
       </c>
       <c r="F3" s="0">
-        <v>0.57306949709480448</v>
+        <v>-0.11062349424238627</v>
       </c>
       <c r="G3" s="0">
-        <v>0.80429083714185357</v>
+        <v>0.0022284809797388123</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.37102404123467009</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4.2888075093408871</v>
+        <v>2.9115312232372008</v>
       </c>
       <c r="B4" s="0">
-        <v>3.5654088056826141</v>
+        <v>2.6564621777071999</v>
       </c>
       <c r="C4" s="0">
-        <v>0.75364944654593802</v>
+        <v>0.50226418826640706</v>
       </c>
       <c r="D4" s="0">
-        <v>0.86812985580841417</v>
+        <v>0.7087059956472832</v>
       </c>
       <c r="E4" s="0">
-        <v>1.003775001599835</v>
+        <v>0.76687707208637412</v>
       </c>
       <c r="F4" s="0">
-        <v>0.24635055345406198</v>
+        <v>0.49773581173359294</v>
       </c>
       <c r="G4" s="0">
-        <v>0.86908494783871282</v>
+        <v>0.7615691800612383</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0.24303265636370625</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>2.1555643126882664</v>
+        <v>3.6717651553544939</v>
       </c>
       <c r="B5" s="0">
-        <v>1.7988757337534982</v>
+        <v>3.3499041146440005</v>
       </c>
       <c r="C5" s="0">
-        <v>0.41250510530319923</v>
+        <v>0.85147151349506167</v>
       </c>
       <c r="D5" s="0">
-        <v>0.64226560339410921</v>
+        <v>0.92275214087807012</v>
       </c>
       <c r="E5" s="0">
-        <v>0.68139232339147637</v>
+        <v>1.0654911306119592</v>
       </c>
       <c r="F5" s="0">
-        <v>0.58749489469680083</v>
+        <v>0.14852848650493833</v>
       </c>
       <c r="G5" s="0">
-        <v>0.8956993287508852</v>
+        <v>0.94024265242527749</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.25012024219036066</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>4.0872285372590085</v>
+        <v>2.1198525763532605</v>
       </c>
       <c r="B6" s="0">
-        <v>3.6333677618357179</v>
+        <v>1.4446834055963067</v>
       </c>
       <c r="C6" s="0">
-        <v>0.50072647998298736</v>
+        <v>0.14116097509208772</v>
       </c>
       <c r="D6" s="0">
-        <v>0.70762029364835721</v>
+        <v>0.37571395381604838</v>
       </c>
       <c r="E6" s="0">
-        <v>0.72205241689899013</v>
+        <v>0.31460875557410856</v>
       </c>
       <c r="F6" s="0">
-        <v>0.49927352001701264</v>
+        <v>0.85883902490791231</v>
       </c>
       <c r="G6" s="0">
-        <v>0.95441200156631067</v>
+        <v>0.93529252501144367</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.12573265577421472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>